<commit_message>
Added error handling integration test
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND01.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND01.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomassw/SOURCE/kainos/NOMS/WMT/wmt-etl/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomassw/SOURCE/kainos/NOMS/WMT/wmt-etl/wmt_etl/tests/data/full_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="31360" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="79">
   <si>
     <t>Trust</t>
   </si>
@@ -164,9 +164,6 @@
     <t>London</t>
   </si>
   <si>
-    <t>LDN</t>
-  </si>
-  <si>
     <t>KainosLDU</t>
   </si>
   <si>
@@ -225,13 +222,61 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>OM_Name</t>
+  </si>
+  <si>
+    <t>Parom_Comp_Last_30</t>
+  </si>
+  <si>
+    <t>Parom_Due_Next_30</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Community</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>NPSQ</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>X555555</t>
+  </si>
+  <si>
+    <t>X444444</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>1001</t>
+  </si>
+  <si>
+    <t>1002</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>ND01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -249,16 +294,43 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -266,17 +338,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCAC9D9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCAC9D9"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCAC9D9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCAC9D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFCAC9D9"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCAC9D9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCAC9D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCAC9D9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCAC9D9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFCAC9D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFCAC9D9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFCAC9D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -554,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AO1" sqref="AO1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -723,28 +863,28 @@
         <v>42</v>
       </c>
       <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>44</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>45</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>46</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>47</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>48</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>49</v>
-      </c>
-      <c r="J2" t="s">
-        <v>50</v>
       </c>
       <c r="K2">
         <v>1001</v>
@@ -848,28 +988,28 @@
         <v>42</v>
       </c>
       <c r="C3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" t="s">
         <v>43</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>44</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>45</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>46</v>
       </c>
-      <c r="G3" t="s">
-        <v>47</v>
-      </c>
       <c r="H3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" t="s">
         <v>51</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>52</v>
-      </c>
-      <c r="J3" t="s">
-        <v>53</v>
       </c>
       <c r="K3">
         <v>1002</v>
@@ -972,60 +1112,104 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" t="s">
         <v>55</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2">
+        <v>1001</v>
+      </c>
+      <c r="E2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="F2">
+        <v>15</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>24</v>
+      </c>
+      <c r="I2" s="3">
+        <v>42795.628472222219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>1002</v>
+      </c>
+      <c r="E3" t="s">
         <v>58</v>
       </c>
-      <c r="B2">
-        <v>15</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3">
+      <c r="F3">
         <v>18</v>
       </c>
-      <c r="C3">
+      <c r="G3">
         <v>11</v>
       </c>
-      <c r="D3">
+      <c r="H3">
         <v>13</v>
+      </c>
+      <c r="I3" s="3">
+        <v>42795.628472222219</v>
       </c>
     </row>
   </sheetData>
@@ -1035,10 +1219,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1047,48 +1231,85 @@
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>55</v>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2">
+        <v>1001</v>
+      </c>
+      <c r="E2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="H2" s="3">
+        <v>42795.628472222219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>1002</v>
+      </c>
+      <c r="E3" t="s">
         <v>58</v>
       </c>
-      <c r="B2">
-        <v>15</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3">
-        <v>18</v>
-      </c>
-      <c r="C3">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>13</v>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3">
+        <v>42795.628472222219</v>
       </c>
     </row>
   </sheetData>
@@ -1098,23 +1319,32 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="A2" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -1126,7 +1356,53 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1136,23 +1412,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -1164,7 +1440,53 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1174,23 +1496,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -1202,7 +1524,53 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1212,23 +1580,23 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -1240,7 +1608,53 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed typo in sample files
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND01.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND01.xlsx
@@ -101,30 +101,6 @@
     <t>CommTierA</t>
   </si>
   <si>
-    <t>LicenseTier0</t>
-  </si>
-  <si>
-    <t>LicenseTierD2</t>
-  </si>
-  <si>
-    <t>LicenseTierD1</t>
-  </si>
-  <si>
-    <t>LicenseTierC2</t>
-  </si>
-  <si>
-    <t>LicenseTierC1</t>
-  </si>
-  <si>
-    <t>LicenseTierB2</t>
-  </si>
-  <si>
-    <t>LicenseTierB1</t>
-  </si>
-  <si>
-    <t>LicenseTierA</t>
-  </si>
-  <si>
     <t>CustTier0</t>
   </si>
   <si>
@@ -270,6 +246,30 @@
   </si>
   <si>
     <t>ND01</t>
+  </si>
+  <si>
+    <t>LicenceTier0</t>
+  </si>
+  <si>
+    <t>LicenceTierD2</t>
+  </si>
+  <si>
+    <t>LicenceTierD1</t>
+  </si>
+  <si>
+    <t>LicenceTierC2</t>
+  </si>
+  <si>
+    <t>LicenceTierC1</t>
+  </si>
+  <si>
+    <t>LicenceTierB2</t>
+  </si>
+  <si>
+    <t>LicenceTierB1</t>
+  </si>
+  <si>
+    <t>LicenceTierA</t>
   </si>
 </sst>
 </file>
@@ -694,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -798,93 +798,93 @@
         <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AF1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AI1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AN1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AO1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
         <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" t="s">
-        <v>49</v>
       </c>
       <c r="K2">
         <v>1001</v>
@@ -982,34 +982,34 @@
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="I3" t="s">
         <v>43</v>
       </c>
-      <c r="E3" t="s">
+      <c r="J3" t="s">
         <v>44</v>
-      </c>
-      <c r="F3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" t="s">
-        <v>52</v>
       </c>
       <c r="K3">
         <v>1002</v>
@@ -1133,42 +1133,42 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D2">
         <v>1001</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F2">
         <v>15</v>
@@ -1185,19 +1185,19 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D3">
         <v>1002</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F3">
         <v>18</v>
@@ -1245,39 +1245,39 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="G1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="H1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D2">
         <v>1001</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -1288,19 +1288,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D3">
         <v>1002</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1338,13 +1338,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -1356,53 +1356,53 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1422,13 +1422,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -1440,53 +1440,53 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="G2" s="4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1506,13 +1506,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -1524,53 +1524,53 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1590,13 +1590,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -1608,53 +1608,53 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update XLSXs to have no blank columns for now
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND01.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND01.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomassw/SOURCE/kainos/NOMS/WMT/wmt-etl/wmt_etl/tests/data/full_inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewwr/src/wmt/etl/wmt_etl/tests/data/full_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -694,7 +694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
@@ -1221,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1280,6 +1280,9 @@
         <v>49</v>
       </c>
       <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
         <v>2</v>
       </c>
       <c r="H2" s="3">

</xml_diff>

<commit_message>
417: Add Jonah Smith
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND01.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="82">
   <si>
     <t>Trust</t>
   </si>
@@ -270,6 +270,15 @@
   </si>
   <si>
     <t>LicenceTierA</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Jonah</t>
+  </si>
+  <si>
+    <t>1003|WMT|C</t>
   </si>
 </sst>
 </file>
@@ -692,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO3"/>
+  <dimension ref="A1:AO4"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1105,6 +1114,131 @@
         <v>42795.628472222219</v>
       </c>
     </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4">
+        <v>1003</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>20</v>
+      </c>
+      <c r="N4">
+        <v>10</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="3">
+        <v>42795.628472222219</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1112,9 +1246,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1212,6 +1348,35 @@
         <v>42795.628472222219</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4">
+        <v>1003</v>
+      </c>
+      <c r="E4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>42795.628472222219</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1219,10 +1384,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1312,6 +1477,32 @@
         <v>1</v>
       </c>
       <c r="H3" s="3">
+        <v>42795.628472222219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4">
+        <v>1003</v>
+      </c>
+      <c r="E4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
         <v>42795.628472222219</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove duplicated OM keys from test data
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND01.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20040" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -703,7 +703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
@@ -1776,7 +1776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
417: Add case details for OM_CODE 1003
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND01.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20040" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="83">
   <si>
     <t>Trust</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t>1003|WMT|C</t>
+  </si>
+  <si>
+    <t>1003</t>
   </si>
 </sst>
 </file>
@@ -703,7 +706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
@@ -1513,10 +1516,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G3"/>
+      <selection activeCell="A4" sqref="A4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1599,6 +1602,29 @@
         <v>59</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1606,10 +1632,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A4" sqref="A4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1683,6 +1709,29 @@
         <v>59</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1690,10 +1739,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1767,6 +1816,29 @@
         <v>59</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1774,10 +1846,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1851,6 +1923,38 @@
         <v>59</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Make ND01.xlsx more realistic based on screenshots
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND01.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND01.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="86">
   <si>
     <t>Trust</t>
   </si>
@@ -282,6 +282,15 @@
   </si>
   <si>
     <t>1003</t>
+  </si>
+  <si>
+    <t>Jonahs LDU</t>
+  </si>
+  <si>
+    <t>JLDU</t>
+  </si>
+  <si>
+    <t>JWMT</t>
   </si>
 </sst>
 </file>
@@ -706,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -902,91 +911,91 @@
         <v>1001</v>
       </c>
       <c r="L2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="O2">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="S2">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="X2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Y2">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="Z2">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="AA2">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="AB2">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="AC2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AD2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AE2">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AF2">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AG2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AH2">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="AI2">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="AJ2">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="AK2">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="AL2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AM2">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AN2">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="AO2" s="3">
         <v>42795.628472222219</v>
@@ -1027,91 +1036,91 @@
         <v>1002</v>
       </c>
       <c r="L3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="N3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O3">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>90</v>
+        <v>2</v>
       </c>
       <c r="U3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="W3">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Y3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Z3">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="AA3">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AB3">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC3">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="AD3">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="AE3">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="AF3">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="AG3">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AH3">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AI3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AJ3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AK3">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="AL3">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AM3">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="AN3">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="AO3" s="3">
         <v>42795.628472222219</v>
@@ -1128,16 +1137,16 @@
         <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="F4" t="s">
         <v>37</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="H4" t="s">
         <v>79</v>
@@ -1155,10 +1164,10 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="N4">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -1167,7 +1176,7 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -1179,7 +1188,7 @@
         <v>0</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V4">
         <v>0</v>
@@ -1188,7 +1197,7 @@
         <v>0</v>
       </c>
       <c r="X4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Y4">
         <v>0</v>
@@ -1519,7 +1528,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G4"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1604,7 +1613,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>63</v>
@@ -1635,7 +1644,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1711,7 +1720,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>63</v>
@@ -1742,7 +1751,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1818,7 +1827,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
989: Adds CMS to test imports and cms table to extract process
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND01.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND01.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewwr/src/wmt/etl/wmt_etl/tests/data/full_inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/terences/Sources/WMT/wmt-etl/wmt_etl/tests/data/full_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Flag_Upw" sheetId="5" r:id="rId5"/>
     <sheet name="Flag_O_Due" sheetId="6" r:id="rId6"/>
     <sheet name="Flag_Priority" sheetId="7" r:id="rId7"/>
+    <sheet name="CMS" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="107">
   <si>
     <t>Trust</t>
   </si>
@@ -291,13 +292,83 @@
   </si>
   <si>
     <t>JWMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact_ID
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact_Date
+</t>
+  </si>
+  <si>
+    <t>Contact_Type_Code</t>
+  </si>
+  <si>
+    <t>Contact_Type_Desc</t>
+  </si>
+  <si>
+    <t>Contact_Staff_Name</t>
+  </si>
+  <si>
+    <t>Contact_Staff_Key</t>
+  </si>
+  <si>
+    <t>Contact_Staff_Grade</t>
+  </si>
+  <si>
+    <t>Contact_Team_Key</t>
+  </si>
+  <si>
+    <t>Contact_Provider_Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OM_Name
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OM_Key
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OM_Grade
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OM_Team_Key
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OM_Provider_Code
+</t>
+  </si>
+  <si>
+    <t>The first type</t>
+  </si>
+  <si>
+    <t>Andy Wright</t>
+  </si>
+  <si>
+    <t>Tom Swann</t>
+  </si>
+  <si>
+    <t>CMS1</t>
+  </si>
+  <si>
+    <t>CMS2</t>
+  </si>
+  <si>
+    <t>The second type</t>
+  </si>
+  <si>
+    <t>Any Wright</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -335,6 +406,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -417,7 +493,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -434,6 +510,13 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -715,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1967,4 +2050,165 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="8" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="9">
+        <v>123</v>
+      </c>
+      <c r="B2" s="10">
+        <v>42991</v>
+      </c>
+      <c r="C2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2">
+        <v>1002</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K2">
+        <v>1001</v>
+      </c>
+      <c r="L2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>321</v>
+      </c>
+      <c r="B3" s="10">
+        <v>42991</v>
+      </c>
+      <c r="C3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F3">
+        <v>1001</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K3">
+        <v>1002</v>
+      </c>
+      <c r="L3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
989: updates test data to include thrid cms reason
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND01.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND01.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="108">
   <si>
     <t>Trust</t>
   </si>
@@ -362,6 +362,9 @@
   </si>
   <si>
     <t>Any Wright</t>
+  </si>
+  <si>
+    <t>CMS3</t>
   </si>
 </sst>
 </file>
@@ -2057,7 +2060,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2216,7 +2219,7 @@
         <v>42991</v>
       </c>
       <c r="C4" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D4" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
977: Update xlsx data
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND01.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND01.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="114">
   <si>
     <t>Trust</t>
   </si>
@@ -378,9 +378,6 @@
   </si>
   <si>
     <t>PO</t>
-  </si>
-  <si>
-    <t>T1</t>
   </si>
   <si>
     <t>Jane Jones</t>
@@ -2287,7 +2284,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2349,13 +2346,13 @@
         <v>110</v>
       </c>
       <c r="F2">
-        <v>1234</v>
+        <v>1003</v>
       </c>
       <c r="G2" t="s">
         <v>111</v>
       </c>
       <c r="H2" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="I2" t="s">
         <v>70</v>
@@ -2375,16 +2372,16 @@
         <v>109</v>
       </c>
       <c r="E3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F3">
-        <v>5678</v>
+        <v>1003</v>
       </c>
       <c r="G3" t="s">
         <v>111</v>
       </c>
       <c r="H3" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="I3" t="s">
         <v>70</v>
@@ -2404,16 +2401,16 @@
         <v>109</v>
       </c>
       <c r="E4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F4">
-        <v>2468</v>
+        <v>1003</v>
       </c>
       <c r="G4" t="s">
         <v>111</v>
       </c>
       <c r="H4" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="I4" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
414: Add ARMS tab to test extract files
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND01.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND01.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/terences/Sources/WMT/wmt-etl/wmt_etl/tests/data/full_inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewwr/src/wmt/etl/wmt_etl/tests/data/full_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Flag_O_Due" sheetId="6" r:id="rId6"/>
     <sheet name="Flag_Priority" sheetId="7" r:id="rId7"/>
     <sheet name="CMS" sheetId="8" r:id="rId8"/>
+    <sheet name="ARMS" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="126">
   <si>
     <t>Trust</t>
   </si>
@@ -365,13 +366,67 @@
   </si>
   <si>
     <t>CMS3</t>
+  </si>
+  <si>
+    <t>Assessment_Date</t>
+  </si>
+  <si>
+    <t>Assessment_Code</t>
+  </si>
+  <si>
+    <t>Assessment_Desc</t>
+  </si>
+  <si>
+    <t>Assessment_Staff_Name</t>
+  </si>
+  <si>
+    <t>Assessment_Staff_Key</t>
+  </si>
+  <si>
+    <t>Assessment_Staff_Grade</t>
+  </si>
+  <si>
+    <t>Assessmentent_Team_Key</t>
+  </si>
+  <si>
+    <t>Assessment_Provider_Code</t>
+  </si>
+  <si>
+    <t>CRN</t>
+  </si>
+  <si>
+    <t>Disposal_or_Release_Date</t>
+  </si>
+  <si>
+    <t>Sentence Type</t>
+  </si>
+  <si>
+    <t>SO_Registration_Date</t>
+  </si>
+  <si>
+    <t>ARMS1</t>
+  </si>
+  <si>
+    <t>Test Arms Assessment</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>C1234567</t>
+  </si>
+  <si>
+    <t>License</t>
+  </si>
+  <si>
+    <t>C1234568</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -415,8 +470,21 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -429,8 +497,20 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0B64A0"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8FBFC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -490,13 +570,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3877A6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3877A6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3877A6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA5A5B1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3877A6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3877A6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA5A5B1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3877A6"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFEBEBEB"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFEBEBEB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFEBEBEB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFEBEBEB"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -520,6 +689,35 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2059,7 +2257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -2258,4 +2456,136 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="18.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="37" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="16">
+        <v>42991</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="19">
+        <v>1002</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" s="16">
+        <v>42991</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="L2" s="16">
+        <v>42991</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="16">
+        <v>42991</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="19">
+        <v>1002</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="J3" s="16">
+        <v>42991</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="16">
+        <v>42991</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
414: Rename `sentence type` to `sentence_type`
We will need to ensure that this is what it will be called in the actual
extract.
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND01.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND01.xlsx
@@ -398,9 +398,6 @@
     <t>Disposal_or_Release_Date</t>
   </si>
   <si>
-    <t>Sentence Type</t>
-  </si>
-  <si>
     <t>SO_Registration_Date</t>
   </si>
   <si>
@@ -420,6 +417,9 @@
   </si>
   <si>
     <t>C1234568</t>
+  </si>
+  <si>
+    <t>Sentence_Type</t>
   </si>
 </sst>
 </file>
@@ -2463,7 +2463,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2503,10 +2503,10 @@
         <v>117</v>
       </c>
       <c r="K1" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="L1" s="14" t="s">
         <v>118</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -2514,10 +2514,10 @@
         <v>42991</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>120</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>121</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>101</v>
@@ -2532,16 +2532,16 @@
         <v>38</v>
       </c>
       <c r="H2" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="I2" s="19" t="s">
         <v>122</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>123</v>
       </c>
       <c r="J2" s="16">
         <v>42991</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L2" s="16">
         <v>42991</v>
@@ -2552,10 +2552,10 @@
         <v>42991</v>
       </c>
       <c r="B3" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>120</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>121</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>101</v>
@@ -2570,10 +2570,10 @@
         <v>38</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J3" s="16">
         <v>42991</v>

</xml_diff>

<commit_message>
977: Update Excel files to use correct GS contact codes
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND01.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND01.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caoimheb/Desktop/Excel files /"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caoimheb/Documents/MOJ_WMT/repos/wmt-etl/wmt_etl/tests/data/full_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="16880" tabRatio="500" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="16880" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="137">
   <si>
     <t>Trust</t>
   </si>
@@ -369,9 +369,6 @@
     <t>CMS3</t>
   </si>
   <si>
-    <t>GS1</t>
-  </si>
-  <si>
     <t>Group supervision</t>
   </si>
   <si>
@@ -448,6 +445,15 @@
   </si>
   <si>
     <t>C1234569</t>
+  </si>
+  <si>
+    <t>NGS004</t>
+  </si>
+  <si>
+    <t>NGS001</t>
+  </si>
+  <si>
+    <t>NGS002</t>
   </si>
 </sst>
 </file>
@@ -1572,7 +1578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:L4"/>
     </sheetView>
   </sheetViews>
@@ -1580,40 +1586,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="37" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="K1" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>124</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1621,10 +1627,10 @@
         <v>42991</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>126</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>127</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>101</v>
@@ -1639,16 +1645,16 @@
         <v>38</v>
       </c>
       <c r="H2" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="19" t="s">
         <v>128</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>129</v>
       </c>
       <c r="J2" s="16">
         <v>42991</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L2" s="16">
         <v>42991</v>
@@ -1659,10 +1665,10 @@
         <v>42991</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>101</v>
@@ -1677,10 +1683,10 @@
         <v>38</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J3" s="16">
         <v>42991</v>
@@ -1697,10 +1703,10 @@
         <v>42991</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>102</v>
@@ -1715,10 +1721,10 @@
         <v>38</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J4" s="16">
         <v>42991</v>
@@ -2657,8 +2663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2711,19 +2717,19 @@
         <v>43033</v>
       </c>
       <c r="C2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" t="s">
         <v>108</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>109</v>
-      </c>
-      <c r="E2" t="s">
-        <v>110</v>
       </c>
       <c r="F2">
         <v>1003</v>
       </c>
       <c r="G2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H2" t="s">
         <v>85</v>
@@ -2740,19 +2746,19 @@
         <v>43033</v>
       </c>
       <c r="C3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" t="s">
         <v>108</v>
       </c>
-      <c r="D3" t="s">
-        <v>109</v>
-      </c>
       <c r="E3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F3">
         <v>1003</v>
       </c>
       <c r="G3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H3" t="s">
         <v>85</v>
@@ -2769,19 +2775,19 @@
         <v>43033</v>
       </c>
       <c r="C4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" t="s">
         <v>108</v>
       </c>
-      <c r="D4" t="s">
-        <v>109</v>
-      </c>
       <c r="E4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F4">
         <v>1003</v>
       </c>
       <c r="G4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H4" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
996: Merge ND0 files
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND01.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND01.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caoimheb/Documents/MOJ_WMT/repos/wmt-etl/wmt_etl/tests/data/full_inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caoimheb/Desktop/Excel files /"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="16880" tabRatio="500" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="16880" tabRatio="500" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,8 @@
     <sheet name="Flag_Priority" sheetId="7" r:id="rId7"/>
     <sheet name="CMS" sheetId="8" r:id="rId8"/>
     <sheet name="GS" sheetId="9" r:id="rId9"/>
-    <sheet name="T2A" sheetId="10" r:id="rId10"/>
+    <sheet name="ARMS" sheetId="10" r:id="rId10"/>
+    <sheet name="T2A" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="137">
   <si>
     <t>Trust</t>
   </si>
@@ -369,9 +370,6 @@
     <t>CMS3</t>
   </si>
   <si>
-    <t>GS1</t>
-  </si>
-  <si>
     <t>Group supervision</t>
   </si>
   <si>
@@ -385,13 +383,85 @@
   </si>
   <si>
     <t>Thomas Boyle</t>
+  </si>
+  <si>
+    <t>Assessment_Date</t>
+  </si>
+  <si>
+    <t>Assessment_Code</t>
+  </si>
+  <si>
+    <t>Assessment_Desc</t>
+  </si>
+  <si>
+    <t>Assessment_Staff_Name</t>
+  </si>
+  <si>
+    <t>Assessment_Staff_Key</t>
+  </si>
+  <si>
+    <t>Assessment_Staff_Grade</t>
+  </si>
+  <si>
+    <t>Assessmentent_Team_Key</t>
+  </si>
+  <si>
+    <t>Assessment_Provider_Code</t>
+  </si>
+  <si>
+    <t>CRN</t>
+  </si>
+  <si>
+    <t>Disposal_or_Release_Date</t>
+  </si>
+  <si>
+    <t>Sentence_Type</t>
+  </si>
+  <si>
+    <t>SO_Registration_Date</t>
+  </si>
+  <si>
+    <t>ARMS1</t>
+  </si>
+  <si>
+    <t>Test Arms Assessment</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>C1234567</t>
+  </si>
+  <si>
+    <t>License</t>
+  </si>
+  <si>
+    <t>ARMS2</t>
+  </si>
+  <si>
+    <t>C1234568</t>
+  </si>
+  <si>
+    <t>ARMS3</t>
+  </si>
+  <si>
+    <t>C1234569</t>
+  </si>
+  <si>
+    <t>NGS004</t>
+  </si>
+  <si>
+    <t>NGS001</t>
+  </si>
+  <si>
+    <t>NGS002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -435,8 +505,21 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -449,8 +532,20 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0B64A0"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8FBFC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -510,13 +605,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3877A6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3877A6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3877A6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA5A5B1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3877A6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3877A6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA5A5B1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3877A6"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFEBEBEB"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFEBEBEB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFEBEBEB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFEBEBEB"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -540,6 +724,36 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="22" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -822,7 +1036,7 @@
   <dimension ref="A1:AO4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="A1:AO4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1364,88 +1578,252 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" ht="37" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="16">
+        <v>42991</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="19">
+        <v>1002</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="J2" s="16">
+        <v>42991</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="L2" s="16">
+        <v>42991</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="16">
+        <v>42991</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="19">
+        <v>1002</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="J3" s="16">
+        <v>42991</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="16">
+        <v>42991</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="16">
+        <v>42991</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="19">
+        <v>1001</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="J4" s="16">
+        <v>42991</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="16">
+        <v>42991</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection sqref="A1:AO4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="41" max="41" width="21.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y1" s="2" t="s">
@@ -1457,16 +1835,16 @@
       <c r="AA1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>77</v>
       </c>
       <c r="AD1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>22</v>
       </c>
       <c r="AF1" s="2" t="s">
@@ -1478,400 +1856,400 @@
       <c r="AH1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" s="2" t="s">
         <v>28</v>
       </c>
       <c r="AL1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="19">
         <v>1001</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="19">
         <v>1</v>
       </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
-      <c r="AB2">
-        <v>0</v>
-      </c>
-      <c r="AC2">
-        <v>0</v>
-      </c>
-      <c r="AD2">
-        <v>0</v>
-      </c>
-      <c r="AE2">
-        <v>0</v>
-      </c>
-      <c r="AF2">
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <v>0</v>
-      </c>
-      <c r="AH2">
-        <v>0</v>
-      </c>
-      <c r="AI2">
-        <v>0</v>
-      </c>
-      <c r="AJ2">
-        <v>0</v>
-      </c>
-      <c r="AK2">
-        <v>0</v>
-      </c>
-      <c r="AL2">
-        <v>0</v>
-      </c>
-      <c r="AM2">
-        <v>0</v>
-      </c>
-      <c r="AN2">
-        <v>0</v>
-      </c>
-      <c r="AO2" s="3">
+      <c r="M2" s="19">
+        <v>0</v>
+      </c>
+      <c r="N2" s="19">
+        <v>0</v>
+      </c>
+      <c r="O2" s="19">
+        <v>0</v>
+      </c>
+      <c r="P2" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="19">
+        <v>0</v>
+      </c>
+      <c r="R2" s="19">
+        <v>0</v>
+      </c>
+      <c r="S2" s="19">
+        <v>0</v>
+      </c>
+      <c r="T2" s="19">
+        <v>0</v>
+      </c>
+      <c r="U2" s="19">
+        <v>0</v>
+      </c>
+      <c r="V2" s="19">
+        <v>0</v>
+      </c>
+      <c r="W2" s="19">
+        <v>0</v>
+      </c>
+      <c r="X2" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="22">
         <v>42795.628472222219</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="19">
         <v>1002</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="19">
         <v>10</v>
       </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>0</v>
-      </c>
-      <c r="AA3">
-        <v>0</v>
-      </c>
-      <c r="AB3">
-        <v>0</v>
-      </c>
-      <c r="AC3">
-        <v>0</v>
-      </c>
-      <c r="AD3">
-        <v>0</v>
-      </c>
-      <c r="AE3">
-        <v>0</v>
-      </c>
-      <c r="AF3">
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <v>0</v>
-      </c>
-      <c r="AH3">
-        <v>0</v>
-      </c>
-      <c r="AI3">
-        <v>0</v>
-      </c>
-      <c r="AJ3">
-        <v>0</v>
-      </c>
-      <c r="AK3">
-        <v>0</v>
-      </c>
-      <c r="AL3">
-        <v>0</v>
-      </c>
-      <c r="AM3">
-        <v>0</v>
-      </c>
-      <c r="AN3">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="3">
+      <c r="M3" s="19">
+        <v>0</v>
+      </c>
+      <c r="N3" s="19">
+        <v>0</v>
+      </c>
+      <c r="O3" s="19">
+        <v>0</v>
+      </c>
+      <c r="P3" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="19">
+        <v>0</v>
+      </c>
+      <c r="R3" s="19">
+        <v>0</v>
+      </c>
+      <c r="S3" s="19">
+        <v>0</v>
+      </c>
+      <c r="T3" s="19">
+        <v>0</v>
+      </c>
+      <c r="U3" s="19">
+        <v>0</v>
+      </c>
+      <c r="V3" s="19">
+        <v>0</v>
+      </c>
+      <c r="W3" s="19">
+        <v>0</v>
+      </c>
+      <c r="X3" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="22">
         <v>42795.628472222219</v>
       </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="19">
         <v>1003</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="19">
         <v>5</v>
       </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4">
-        <v>0</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
-      <c r="AB4">
-        <v>0</v>
-      </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
-      <c r="AD4">
-        <v>0</v>
-      </c>
-      <c r="AE4">
-        <v>0</v>
-      </c>
-      <c r="AF4">
-        <v>0</v>
-      </c>
-      <c r="AG4">
-        <v>0</v>
-      </c>
-      <c r="AH4">
-        <v>0</v>
-      </c>
-      <c r="AI4">
-        <v>0</v>
-      </c>
-      <c r="AJ4">
-        <v>0</v>
-      </c>
-      <c r="AK4">
-        <v>0</v>
-      </c>
-      <c r="AL4">
-        <v>0</v>
-      </c>
-      <c r="AM4">
-        <v>0</v>
-      </c>
-      <c r="AN4">
-        <v>0</v>
-      </c>
-      <c r="AO4" s="3">
+      <c r="M4" s="19">
+        <v>0</v>
+      </c>
+      <c r="N4" s="19">
+        <v>0</v>
+      </c>
+      <c r="O4" s="19">
+        <v>0</v>
+      </c>
+      <c r="P4" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="19">
+        <v>0</v>
+      </c>
+      <c r="R4" s="19">
+        <v>0</v>
+      </c>
+      <c r="S4" s="19">
+        <v>0</v>
+      </c>
+      <c r="T4" s="19">
+        <v>0</v>
+      </c>
+      <c r="U4" s="19">
+        <v>0</v>
+      </c>
+      <c r="V4" s="19">
+        <v>0</v>
+      </c>
+      <c r="W4" s="19">
+        <v>0</v>
+      </c>
+      <c r="X4" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="22">
         <v>42795.628472222219</v>
       </c>
     </row>
@@ -2803,7 +3181,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2856,19 +3234,19 @@
         <v>43033</v>
       </c>
       <c r="C2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" t="s">
         <v>108</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>109</v>
-      </c>
-      <c r="E2" t="s">
-        <v>110</v>
       </c>
       <c r="F2">
         <v>1003</v>
       </c>
       <c r="G2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H2" t="s">
         <v>85</v>
@@ -2885,19 +3263,19 @@
         <v>43033</v>
       </c>
       <c r="C3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" t="s">
         <v>108</v>
       </c>
-      <c r="D3" t="s">
-        <v>109</v>
-      </c>
       <c r="E3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F3">
         <v>1003</v>
       </c>
       <c r="G3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H3" t="s">
         <v>85</v>
@@ -2914,19 +3292,19 @@
         <v>43033</v>
       </c>
       <c r="C4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" t="s">
         <v>108</v>
       </c>
-      <c r="D4" t="s">
-        <v>109</v>
-      </c>
       <c r="E4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F4">
         <v>1003</v>
       </c>
       <c r="G4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H4" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
Update data in excel spreadsheet to illustrate e2e pipeline
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND01.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="16880" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="16880" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="134">
   <si>
     <t>Trust</t>
   </si>
@@ -372,16 +372,7 @@
     <t>Group supervision</t>
   </si>
   <si>
-    <t>Billy Jones</t>
-  </si>
-  <si>
     <t>PO</t>
-  </si>
-  <si>
-    <t>Jane Jones</t>
-  </si>
-  <si>
-    <t>Thomas Boyle</t>
   </si>
   <si>
     <t>Assessment_Date</t>
@@ -694,8 +685,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -753,9 +746,11 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1586,40 +1581,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="37" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="I1" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="J1" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="K1" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>121</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1627,10 +1622,10 @@
         <v>42991</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>101</v>
@@ -1645,16 +1640,16 @@
         <v>38</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J2" s="16">
         <v>42991</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L2" s="16">
         <v>42991</v>
@@ -1665,10 +1660,10 @@
         <v>42991</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>101</v>
@@ -1683,10 +1678,10 @@
         <v>38</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="J3" s="16">
         <v>42991</v>
@@ -1703,10 +1698,10 @@
         <v>42991</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>102</v>
@@ -1721,10 +1716,10 @@
         <v>38</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="J4" s="16">
         <v>42991</v>
@@ -2458,8 +2453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2527,7 +2522,7 @@
         <v>123</v>
       </c>
       <c r="B2" s="10">
-        <v>42991</v>
+        <v>43021</v>
       </c>
       <c r="C2" t="s">
         <v>103</v>
@@ -2571,7 +2566,7 @@
         <v>321</v>
       </c>
       <c r="B3" s="10">
-        <v>42991</v>
+        <v>43021</v>
       </c>
       <c r="C3" t="s">
         <v>104</v>
@@ -2615,7 +2610,7 @@
         <v>456</v>
       </c>
       <c r="B4" s="10">
-        <v>42991</v>
+        <v>43021</v>
       </c>
       <c r="C4" t="s">
         <v>107</v>
@@ -2663,17 +2658,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" customWidth="1"/>
     <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
@@ -2717,22 +2712,22 @@
         <v>43033</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D2" t="s">
         <v>108</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="19">
+        <v>1002</v>
+      </c>
+      <c r="G2" t="s">
         <v>109</v>
       </c>
-      <c r="F2">
-        <v>1003</v>
-      </c>
-      <c r="G2" t="s">
-        <v>110</v>
-      </c>
       <c r="H2" t="s">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s">
         <v>70</v>
@@ -2746,22 +2741,22 @@
         <v>43033</v>
       </c>
       <c r="C3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D3" t="s">
         <v>108</v>
       </c>
-      <c r="E3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F3">
-        <v>1003</v>
+      <c r="E3" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F3" s="19">
+        <v>1001</v>
       </c>
       <c r="G3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H3" t="s">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="I3" t="s">
         <v>70</v>
@@ -2775,22 +2770,22 @@
         <v>43033</v>
       </c>
       <c r="C4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D4" t="s">
         <v>108</v>
       </c>
-      <c r="E4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F4">
-        <v>1003</v>
+      <c r="E4" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" s="19">
+        <v>1002</v>
       </c>
       <c r="G4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H4" t="s">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="I4" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
996: Merge from master
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND01.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND01.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caoimheb/Desktop/Excel files /"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caoimheb/Documents/MOJ_WMT/repos/wmt-etl/wmt_etl/tests/data/full_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="16880" tabRatio="500" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="16880" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,6 @@
     <sheet name="CMS" sheetId="8" r:id="rId8"/>
     <sheet name="GS" sheetId="9" r:id="rId9"/>
     <sheet name="ARMS" sheetId="10" r:id="rId10"/>
-    <sheet name="T2A" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="134">
   <si>
     <t>Trust</t>
   </si>
@@ -373,16 +372,7 @@
     <t>Group supervision</t>
   </si>
   <si>
-    <t>Billy Jones</t>
-  </si>
-  <si>
     <t>PO</t>
-  </si>
-  <si>
-    <t>Jane Jones</t>
-  </si>
-  <si>
-    <t>Thomas Boyle</t>
   </si>
   <si>
     <t>Assessment_Date</t>
@@ -695,12 +685,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -753,11 +745,12 @@
     <xf numFmtId="49" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="22" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1588,40 +1581,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="37" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="I1" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="J1" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="K1" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>121</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1629,10 +1622,10 @@
         <v>42991</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>101</v>
@@ -1647,16 +1640,16 @@
         <v>38</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J2" s="16">
         <v>42991</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L2" s="16">
         <v>42991</v>
@@ -1667,10 +1660,10 @@
         <v>42991</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>101</v>
@@ -1685,10 +1678,10 @@
         <v>38</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="J3" s="16">
         <v>42991</v>
@@ -1705,10 +1698,10 @@
         <v>42991</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>102</v>
@@ -1723,10 +1716,10 @@
         <v>38</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="J4" s="16">
         <v>42991</v>
@@ -1736,521 +1729,6 @@
       </c>
       <c r="L4" s="16">
         <v>42991</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AO4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:41" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" s="19">
-        <v>1001</v>
-      </c>
-      <c r="L2" s="19">
-        <v>1</v>
-      </c>
-      <c r="M2" s="19">
-        <v>0</v>
-      </c>
-      <c r="N2" s="19">
-        <v>0</v>
-      </c>
-      <c r="O2" s="19">
-        <v>0</v>
-      </c>
-      <c r="P2" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="19">
-        <v>0</v>
-      </c>
-      <c r="R2" s="19">
-        <v>0</v>
-      </c>
-      <c r="S2" s="19">
-        <v>0</v>
-      </c>
-      <c r="T2" s="19">
-        <v>0</v>
-      </c>
-      <c r="U2" s="19">
-        <v>0</v>
-      </c>
-      <c r="V2" s="19">
-        <v>0</v>
-      </c>
-      <c r="W2" s="19">
-        <v>0</v>
-      </c>
-      <c r="X2" s="19">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="19">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AE2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AG2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AI2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AM2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AN2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AO2" s="22">
-        <v>42795.628472222219</v>
-      </c>
-    </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="K3" s="19">
-        <v>1002</v>
-      </c>
-      <c r="L3" s="19">
-        <v>10</v>
-      </c>
-      <c r="M3" s="19">
-        <v>0</v>
-      </c>
-      <c r="N3" s="19">
-        <v>0</v>
-      </c>
-      <c r="O3" s="19">
-        <v>0</v>
-      </c>
-      <c r="P3" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="19">
-        <v>0</v>
-      </c>
-      <c r="R3" s="19">
-        <v>0</v>
-      </c>
-      <c r="S3" s="19">
-        <v>0</v>
-      </c>
-      <c r="T3" s="19">
-        <v>0</v>
-      </c>
-      <c r="U3" s="19">
-        <v>0</v>
-      </c>
-      <c r="V3" s="19">
-        <v>0</v>
-      </c>
-      <c r="W3" s="19">
-        <v>0</v>
-      </c>
-      <c r="X3" s="19">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="19">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="19">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="22">
-        <v>42795.628472222219</v>
-      </c>
-    </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="I4" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="J4" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="K4" s="19">
-        <v>1003</v>
-      </c>
-      <c r="L4" s="19">
-        <v>5</v>
-      </c>
-      <c r="M4" s="19">
-        <v>0</v>
-      </c>
-      <c r="N4" s="19">
-        <v>0</v>
-      </c>
-      <c r="O4" s="19">
-        <v>0</v>
-      </c>
-      <c r="P4" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="19">
-        <v>0</v>
-      </c>
-      <c r="R4" s="19">
-        <v>0</v>
-      </c>
-      <c r="S4" s="19">
-        <v>0</v>
-      </c>
-      <c r="T4" s="19">
-        <v>0</v>
-      </c>
-      <c r="U4" s="19">
-        <v>0</v>
-      </c>
-      <c r="V4" s="19">
-        <v>0</v>
-      </c>
-      <c r="W4" s="19">
-        <v>0</v>
-      </c>
-      <c r="X4" s="19">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="19">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AJ4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AL4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AM4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AN4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AO4" s="22">
-        <v>42795.628472222219</v>
       </c>
     </row>
   </sheetData>
@@ -2975,8 +2453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3044,7 +2522,7 @@
         <v>123</v>
       </c>
       <c r="B2" s="10">
-        <v>42991</v>
+        <v>43021</v>
       </c>
       <c r="C2" t="s">
         <v>103</v>
@@ -3088,7 +2566,7 @@
         <v>321</v>
       </c>
       <c r="B3" s="10">
-        <v>42991</v>
+        <v>43021</v>
       </c>
       <c r="C3" t="s">
         <v>104</v>
@@ -3132,7 +2610,7 @@
         <v>456</v>
       </c>
       <c r="B4" s="10">
-        <v>42991</v>
+        <v>43021</v>
       </c>
       <c r="C4" t="s">
         <v>107</v>
@@ -3181,16 +2659,16 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" customWidth="1"/>
     <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
@@ -3234,22 +2712,22 @@
         <v>43033</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D2" t="s">
         <v>108</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="19">
+        <v>1002</v>
+      </c>
+      <c r="G2" t="s">
         <v>109</v>
       </c>
-      <c r="F2">
-        <v>1003</v>
-      </c>
-      <c r="G2" t="s">
-        <v>110</v>
-      </c>
       <c r="H2" t="s">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s">
         <v>70</v>
@@ -3263,22 +2741,22 @@
         <v>43033</v>
       </c>
       <c r="C3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D3" t="s">
         <v>108</v>
       </c>
-      <c r="E3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F3">
-        <v>1003</v>
+      <c r="E3" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F3" s="19">
+        <v>1001</v>
       </c>
       <c r="G3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H3" t="s">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="I3" t="s">
         <v>70</v>
@@ -3292,22 +2770,22 @@
         <v>43033</v>
       </c>
       <c r="C4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D4" t="s">
         <v>108</v>
       </c>
-      <c r="E4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F4">
-        <v>1003</v>
+      <c r="E4" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" s="19">
+        <v>1002</v>
       </c>
       <c r="G4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H4" t="s">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="I4" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
175: Update test data for court reports
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND01.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="16880" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="1820" yWindow="7280" windowWidth="29100" windowHeight="10600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="147">
   <si>
     <t>Trust</t>
   </si>
@@ -445,13 +445,54 @@
   </si>
   <si>
     <t>NGS002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDU_Code
+</t>
+  </si>
+  <si>
+    <t>LDU_Desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oral_reports
+</t>
+  </si>
+  <si>
+    <t>Court</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Simon</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>2002|WMT|C</t>
+  </si>
+  <si>
+    <t>2001|WMT|Z</t>
+  </si>
+  <si>
+    <t>CRP</t>
+  </si>
+  <si>
+    <t>CR Team</t>
+  </si>
+  <si>
+    <t>CRLDU</t>
+  </si>
+  <si>
+    <t>CR LDU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -508,8 +549,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="9"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -534,8 +586,20 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="54"/>
+        <bgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -684,6 +748,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="31"/>
+      </left>
+      <right style="thin">
+        <color indexed="31"/>
+      </right>
+      <top style="thin">
+        <color indexed="31"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="31"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -692,7 +771,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -743,6 +822,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1026,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO4"/>
+  <dimension ref="A1:AP4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1039,7 +1127,7 @@
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
     <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.1640625" bestFit="1" customWidth="1"/>
@@ -1064,7 +1152,7 @@
     <col min="41" max="41" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1188,8 +1276,9 @@
       <c r="AO1" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP1" s="1"/>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1314,7 +1403,7 @@
         <v>42795.628472222219</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1439,7 +1528,7 @@
         <v>42795.628472222219</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -1573,13 +1662,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L4"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="37" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="25" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>110</v>
       </c>
@@ -1738,134 +1838,350 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:AO6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.33203125" customWidth="1"/>
+    <col min="18" max="40" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:41" s="24" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="H1" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F1" t="s">
+      <c r="M1" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="G1" t="s">
+      <c r="N1" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="H1" t="s">
+      <c r="O1" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="I1" t="s">
+      <c r="P1" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q1" s="23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
         <v>39</v>
       </c>
-      <c r="D2">
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2">
         <v>1001</v>
       </c>
-      <c r="E2" t="s">
+      <c r="K2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" t="s">
         <v>49</v>
       </c>
-      <c r="F2">
-        <v>15</v>
-      </c>
-      <c r="G2">
+      <c r="M2">
         <v>5</v>
       </c>
-      <c r="H2">
-        <v>24</v>
-      </c>
-      <c r="I2" s="3">
+      <c r="N2">
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <v>3</v>
+      </c>
+      <c r="P2">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="3">
         <v>42795.628472222219</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="AO2" s="3"/>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
         <v>37</v>
       </c>
-      <c r="B3" t="s">
+      <c r="G3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" t="s">
+      <c r="H3" t="s">
         <v>42</v>
       </c>
-      <c r="D3">
+      <c r="I3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3">
         <v>1002</v>
       </c>
-      <c r="E3" t="s">
+      <c r="K3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" t="s">
         <v>50</v>
       </c>
-      <c r="F3">
-        <v>18</v>
-      </c>
-      <c r="G3">
-        <v>11</v>
-      </c>
-      <c r="H3">
-        <v>13</v>
-      </c>
-      <c r="I3" s="3">
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>5</v>
+      </c>
+      <c r="P3">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="3">
         <v>42795.628472222219</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" t="s">
         <v>37</v>
       </c>
-      <c r="B4" t="s">
+      <c r="G4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J4">
+        <v>1003</v>
+      </c>
+      <c r="K4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" t="s">
+        <v>81</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="O4">
+        <v>6</v>
+      </c>
+      <c r="P4">
+        <v>8</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>42795.628472222219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
         <v>38</v>
       </c>
-      <c r="C4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4">
-        <v>1003</v>
-      </c>
-      <c r="E4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3">
+      <c r="H5" t="s">
+        <v>137</v>
+      </c>
+      <c r="I5" t="s">
+        <v>138</v>
+      </c>
+      <c r="J5">
+        <v>2001</v>
+      </c>
+      <c r="K5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" t="s">
+        <v>142</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5">
+        <v>5</v>
+      </c>
+      <c r="P5">
+        <v>7</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>42795.628472222219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" t="s">
+        <v>145</v>
+      </c>
+      <c r="F6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H6" t="s">
+        <v>140</v>
+      </c>
+      <c r="I6" t="s">
+        <v>139</v>
+      </c>
+      <c r="J6">
+        <v>2002</v>
+      </c>
+      <c r="K6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" t="s">
+        <v>141</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6">
+        <v>6</v>
+      </c>
+      <c r="P6">
+        <v>8</v>
+      </c>
+      <c r="Q6" s="3">
         <v>42795.628472222219</v>
       </c>
     </row>
@@ -2453,7 +2769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
996: Merge back T2A sheet in the test files
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND01.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND01.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caoimheb/Documents/MOJ_WMT/repos/wmt-etl/wmt_etl/tests/data/full_inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derejed/Projects/HMMPS/wmt-etl/wmt_etl/tests/data/full_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="16880" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="-3780" yWindow="-18560" windowWidth="28800" windowHeight="16480" tabRatio="500" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="CMS" sheetId="8" r:id="rId8"/>
     <sheet name="GS" sheetId="9" r:id="rId9"/>
     <sheet name="ARMS" sheetId="10" r:id="rId10"/>
+    <sheet name="T2A" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="134">
   <si>
     <t>Trust</t>
   </si>
@@ -692,7 +693,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -745,6 +746,7 @@
     <xf numFmtId="49" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="22" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1736,6 +1738,521 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AO4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:AO4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:41" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="19">
+        <v>1001</v>
+      </c>
+      <c r="L2" s="19">
+        <v>1</v>
+      </c>
+      <c r="M2" s="19">
+        <v>0</v>
+      </c>
+      <c r="N2" s="19">
+        <v>0</v>
+      </c>
+      <c r="O2" s="19">
+        <v>0</v>
+      </c>
+      <c r="P2" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="19">
+        <v>0</v>
+      </c>
+      <c r="R2" s="19">
+        <v>0</v>
+      </c>
+      <c r="S2" s="19">
+        <v>0</v>
+      </c>
+      <c r="T2" s="19">
+        <v>0</v>
+      </c>
+      <c r="U2" s="19">
+        <v>0</v>
+      </c>
+      <c r="V2" s="19">
+        <v>0</v>
+      </c>
+      <c r="W2" s="19">
+        <v>0</v>
+      </c>
+      <c r="X2" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="22">
+        <v>42795.628472222219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="19">
+        <v>1002</v>
+      </c>
+      <c r="L3" s="19">
+        <v>10</v>
+      </c>
+      <c r="M3" s="19">
+        <v>0</v>
+      </c>
+      <c r="N3" s="19">
+        <v>0</v>
+      </c>
+      <c r="O3" s="19">
+        <v>0</v>
+      </c>
+      <c r="P3" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="19">
+        <v>0</v>
+      </c>
+      <c r="R3" s="19">
+        <v>0</v>
+      </c>
+      <c r="S3" s="19">
+        <v>0</v>
+      </c>
+      <c r="T3" s="19">
+        <v>0</v>
+      </c>
+      <c r="U3" s="19">
+        <v>0</v>
+      </c>
+      <c r="V3" s="19">
+        <v>0</v>
+      </c>
+      <c r="W3" s="19">
+        <v>0</v>
+      </c>
+      <c r="X3" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="19">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="22">
+        <v>42795.628472222219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="19">
+        <v>1003</v>
+      </c>
+      <c r="L4" s="19">
+        <v>5</v>
+      </c>
+      <c r="M4" s="19">
+        <v>0</v>
+      </c>
+      <c r="N4" s="19">
+        <v>0</v>
+      </c>
+      <c r="O4" s="19">
+        <v>0</v>
+      </c>
+      <c r="P4" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="19">
+        <v>0</v>
+      </c>
+      <c r="R4" s="19">
+        <v>0</v>
+      </c>
+      <c r="S4" s="19">
+        <v>0</v>
+      </c>
+      <c r="T4" s="19">
+        <v>0</v>
+      </c>
+      <c r="U4" s="19">
+        <v>0</v>
+      </c>
+      <c r="V4" s="19">
+        <v>0</v>
+      </c>
+      <c r="W4" s="19">
+        <v>0</v>
+      </c>
+      <c r="X4" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="22">
+        <v>42795.628472222219</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
@@ -2453,7 +2970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
408: Add data for wmt_extract_sa tab
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND01.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND01.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="152">
   <si>
     <t>Trust</t>
   </si>
@@ -467,13 +467,49 @@
   </si>
   <si>
     <t>Standalone_Order</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>ORA Suspended Sentence Order</t>
+  </si>
+  <si>
+    <t>SA Curfew</t>
+  </si>
+  <si>
+    <t>Custody</t>
+  </si>
+  <si>
+    <t>ORA Community Order</t>
+  </si>
+  <si>
+    <t>SA Electronic Monitoring</t>
+  </si>
+  <si>
+    <t>D42237</t>
+  </si>
+  <si>
+    <t>D42371</t>
+  </si>
+  <si>
+    <t>D50370</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>CJA - Suspended Sentence Order</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -540,6 +576,19 @@
       <sz val="6"/>
       <color indexed="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -745,14 +794,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -815,12 +866,28 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="22" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1098,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1823,7 +1890,7 @@
   <dimension ref="A1:AO4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:AO4"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2335,42 +2402,252 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.5" style="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="30"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="24" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:10" s="27" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="26" t="s">
         <v>139</v>
       </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="J2" s="29"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="J3" s="29"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="J4" s="29"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="29"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="29"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="29"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="29"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="29"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="29"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="29"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update field name -> Assessment_Team_Key
</commit_message>
<xml_diff>
--- a/wmt_etl/tests/data/full_inputs/ND01.xlsx
+++ b/wmt_etl/tests/data/full_inputs/ND01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="3700" windowWidth="29100" windowHeight="10600" tabRatio="500" activeTab="11"/>
+    <workbookView xWindow="1720" yWindow="3700" windowWidth="29100" windowHeight="10600" tabRatio="500" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="WMT_Extract" sheetId="1" r:id="rId1"/>
@@ -395,9 +395,6 @@
     <t>Assessment_Staff_Grade</t>
   </si>
   <si>
-    <t>Assessmentent_Team_Key</t>
-  </si>
-  <si>
     <t>Assessment_Provider_Code</t>
   </si>
   <si>
@@ -503,6 +500,9 @@
   </si>
   <si>
     <t>CJA - Suspended Sentence Order</t>
+  </si>
+  <si>
+    <t>Assessment_Team_Key</t>
   </si>
 </sst>
 </file>
@@ -1711,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1748,22 +1748,22 @@
         <v>115</v>
       </c>
       <c r="G1" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="K1" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>120</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1771,10 +1771,10 @@
         <v>42991</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>122</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>123</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>101</v>
@@ -1789,16 +1789,16 @@
         <v>38</v>
       </c>
       <c r="H2" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" s="19" t="s">
         <v>124</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>125</v>
       </c>
       <c r="J2" s="16">
         <v>42991</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L2" s="16">
         <v>42991</v>
@@ -1809,10 +1809,10 @@
         <v>42991</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>101</v>
@@ -1827,10 +1827,10 @@
         <v>38</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J3" s="16">
         <v>42991</v>
@@ -1847,10 +1847,10 @@
         <v>42991</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>102</v>
@@ -1865,10 +1865,10 @@
         <v>38</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J4" s="16">
         <v>42991</v>
@@ -2404,7 +2404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -2442,21 +2442,21 @@
         <v>54</v>
       </c>
       <c r="G1" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="I1" s="26" t="s">
         <v>138</v>
-      </c>
-      <c r="I1" s="26" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>38</v>
@@ -2471,19 +2471,19 @@
         <v>59</v>
       </c>
       <c r="G2" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="I2" s="28" t="s">
         <v>141</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>142</v>
       </c>
       <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B3" s="28" t="s">
         <v>60</v>
@@ -2501,19 +2501,19 @@
         <v>59</v>
       </c>
       <c r="G3" s="31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I3" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J3" s="29"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B4" s="28" t="s">
         <v>60</v>
@@ -2528,16 +2528,16 @@
         <v>66</v>
       </c>
       <c r="F4" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="G4" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="H4" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="I4" s="28" t="s">
         <v>144</v>
-      </c>
-      <c r="H4" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="I4" s="28" t="s">
-        <v>145</v>
       </c>
       <c r="J4" s="29"/>
     </row>
@@ -2695,10 +2695,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F1" s="23" t="s">
         <v>5</v>
@@ -2731,7 +2731,7 @@
         <v>48</v>
       </c>
       <c r="P1" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Q1" s="23" t="s">
         <v>32</v>
@@ -3746,7 +3746,7 @@
         <v>43033</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
         <v>108</v>
@@ -3775,7 +3775,7 @@
         <v>43033</v>
       </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D3" t="s">
         <v>108</v>
@@ -3804,7 +3804,7 @@
         <v>43033</v>
       </c>
       <c r="C4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D4" t="s">
         <v>108</v>

</xml_diff>